<commit_message>
feat: Implementación completa del módulo de logística
- Agregado sistema de autenticación SSO con portal central
- Implementado dashboard con estadísticas y navegación interactiva
- Creado páginas para gestión de productos, recepciones, despachos
- Agregado sistema de ordenamiento (put-away) y control de inventario
- Implementado gestión de proyectos, proveedores y bodegas
- Integrado WMSTopBar para navegación consistente
- Configurado layout limpio sin sidebars duplicados
- Agregado soporte para roles de logística en el backend
</commit_message>
<xml_diff>
--- a/public/inventario.xlsx
+++ b/public/inventario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosalegria/Desktop/informe Telefonica/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosalegria/Desktop/Aplicaciones Carlos Alegria/PORTAL_SOMYL_2026/modulo_logistica/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E81802-4B20-D547-BFC2-5F6219084B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594E11FF-D4D2-F84D-96AB-FB66B9D2BC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840" xr2:uid="{C5E3BA87-039D-EC49-8A7D-F58DA0CE356F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" xr2:uid="{C5E3BA87-039D-EC49-8A7D-F58DA0CE356F}"/>
   </bookViews>
   <sheets>
     <sheet name="MAESTRO" sheetId="1" r:id="rId1"/>
@@ -677,10 +677,10 @@
   <dimension ref="A1:I412"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H120" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="J379" sqref="J379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8264,7 +8264,7 @@
         <v>8</v>
       </c>
       <c r="I402" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="403" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>